<commit_message>
Changes made by Rahul
</commit_message>
<xml_diff>
--- a/crowdStaffingAPIs.xlsx
+++ b/crowdStaffingAPIs.xlsx
@@ -1144,8 +1144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1173,7 +1173,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>34</v>
       </c>
@@ -1183,7 +1183,7 @@
       <c r="C4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="15" t="s">
         <v>1</v>
       </c>
       <c r="E4" s="9" t="s">

</xml_diff>